<commit_message>
Rapta-C constraints list completed
</commit_message>
<xml_diff>
--- a/Data/Compound Constraints/Compounds Ub RAPTA-C.xlsx
+++ b/Data/Compound Constraints/Compounds Ub RAPTA-C.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MatthewMBP/Dropbox (Uni of Auckland)/Research/Comp sci project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hasnaij\Desktop\Compsci380\MLMSA\Data\Compound Constraints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AECC5A56-546C-EE47-84AB-F6BBFFAE1D8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5049264-0247-49EF-A0F3-D7A507388AFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6400" yWindow="460" windowWidth="25600" windowHeight="14320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -427,18 +427,18 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -458,7 +458,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -478,7 +478,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f>A2+1</f>
         <v>2</v>
@@ -499,7 +499,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f>A3+1</f>
         <v>3</v>
@@ -510,6 +510,9 @@
       <c r="C4" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="D4" s="1">
+        <v>102.911626</v>
+      </c>
       <c r="E4" s="1">
         <v>0</v>
       </c>
@@ -517,9 +520,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <f t="shared" ref="A5:A13" si="0">A4+1</f>
+        <f t="shared" ref="A5:A10" si="0">A4+1</f>
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -538,7 +541,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -559,7 +562,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -580,7 +583,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -591,6 +594,9 @@
       <c r="C8" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="D8" s="1">
+        <v>135.116827</v>
+      </c>
       <c r="E8" s="1">
         <v>0</v>
       </c>
@@ -598,7 +604,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -609,6 +615,9 @@
       <c r="C9" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="D9" s="1">
+        <v>158.08416</v>
+      </c>
       <c r="E9" s="1">
         <v>0</v>
       </c>
@@ -616,7 +625,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -637,7 +646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F16" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Results and System 3 demo push
</commit_message>
<xml_diff>
--- a/Data/Compound Constraints/Compounds Ub RAPTA-C.xlsx
+++ b/Data/Compound Constraints/Compounds Ub RAPTA-C.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hasnaij\Desktop\Compsci380\MLMSA\Data\Compound Constraints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5049264-0247-49EF-A0F3-D7A507388AFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{873A0CA8-97BC-49A3-930D-864DE99F3A34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36000" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -427,7 +427,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>